<commit_message>
Script & Test Data changes
</commit_message>
<xml_diff>
--- a/TestData/TestDataFile.xlsx
+++ b/TestData/TestDataFile.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="11">
   <si>
     <t>Item</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Pick up at store</t>
+  </si>
+  <si>
+    <t>88011944</t>
   </si>
 </sst>
 </file>
@@ -417,18 +420,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H3"/>
+      <selection activeCell="A4" sqref="A4:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.140625" customWidth="1"/>
+    <col min="2" max="3" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="15.140625" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="21.5703125" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="16.140625" customWidth="1" collapsed="1"/>
   </cols>
@@ -502,9 +504,6 @@
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -542,7 +541,7 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
@@ -602,7 +601,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="A4" sqref="A4:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated at 2:08 PM
</commit_message>
<xml_diff>
--- a/TestData/TestDataFile.xlsx
+++ b/TestData/TestDataFile.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView activeTab="2" windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="BOPIS_TestData" sheetId="1" r:id="rId1"/>
-    <sheet name="SFS_TestData" sheetId="2" r:id="rId2"/>
-    <sheet name="STS_TestData" sheetId="3" r:id="rId3"/>
+    <sheet name="BOPIS_TestData" r:id="rId1" sheetId="1"/>
+    <sheet name="SFS_TestData" r:id="rId2" sheetId="2"/>
+    <sheet name="STS_TestData" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
   <si>
     <t>Item</t>
   </si>
@@ -54,12 +54,28 @@
   </si>
   <si>
     <t>88011944</t>
+  </si>
+  <si>
+    <t>88011951</t>
+  </si>
+  <si>
+    <t>88011952</t>
+  </si>
+  <si>
+    <t>88011953</t>
+  </si>
+  <si>
+    <t>88011954</t>
+  </si>
+  <si>
+    <t>88011955</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -129,23 +145,23 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -162,10 +178,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -200,7 +216,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -235,7 +251,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -329,21 +345,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -360,7 +376,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -412,14 +428,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -428,11 +444,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -455,13 +471,13 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -506,13 +522,13 @@
       <c r="H3" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -541,7 +557,7 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
@@ -592,12 +608,12 @@
       <c r="H3" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -626,7 +642,7 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
@@ -677,6 +693,6 @@
       <c r="H3" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated screenshot save path
</commit_message>
<xml_diff>
--- a/TestData/TestDataFile.xlsx
+++ b/TestData/TestDataFile.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="BOPIS_TestData" sheetId="1" r:id="rId1"/>
-    <sheet name="SFS_TestData" sheetId="2" r:id="rId2"/>
-    <sheet name="STS_TestData" sheetId="3" r:id="rId3"/>
-    <sheet name="BackUp" sheetId="4" r:id="rId4"/>
+    <sheet name="BOPIS_TestData" r:id="rId1" sheetId="1"/>
+    <sheet name="SFS_TestData" r:id="rId2" sheetId="2"/>
+    <sheet name="STS_TestData" r:id="rId3" sheetId="3"/>
+    <sheet name="BackUp" r:id="rId4" sheetId="4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="13">
   <si>
     <t>Item</t>
   </si>
@@ -58,12 +58,16 @@
   </si>
   <si>
     <t>88012146</t>
+  </si>
+  <si>
+    <t>88012153</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -133,23 +137,23 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -166,10 +170,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -204,7 +208,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -239,7 +243,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -333,21 +337,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -364,7 +368,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -416,14 +420,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -432,11 +436,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -465,7 +469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -485,16 +489,18 @@
         <v>18052</v>
       </c>
       <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -503,8 +509,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -580,12 +586,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -594,7 +600,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -648,12 +654,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -733,6 +739,6 @@
       <c r="H3" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test Data - Updated
</commit_message>
<xml_diff>
--- a/TestData/TestDataFile.xlsx
+++ b/TestData/TestDataFile.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="BOPIS_TestData" r:id="rId1" sheetId="1"/>
-    <sheet name="SFS_TestData" r:id="rId2" sheetId="2"/>
-    <sheet name="STS_TestData" r:id="rId3" sheetId="3"/>
-    <sheet name="BackUp" r:id="rId4" sheetId="4"/>
+    <sheet name="BOPIS_TestData" sheetId="1" r:id="rId1"/>
+    <sheet name="SFS_TestData" sheetId="2" r:id="rId2"/>
+    <sheet name="STS_TestData" sheetId="3" r:id="rId3"/>
+    <sheet name="BackUp" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="13">
   <si>
     <t>Item</t>
   </si>
@@ -54,64 +54,10 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>88012143</t>
-  </si>
-  <si>
-    <t>88012146</t>
-  </si>
-  <si>
-    <t>88012258</t>
-  </si>
-  <si>
-    <t>88012272</t>
-  </si>
-  <si>
-    <t>88012335</t>
-  </si>
-  <si>
-    <t>88012336</t>
-  </si>
-  <si>
-    <t>88012469</t>
-  </si>
-  <si>
-    <t>88012485</t>
-  </si>
-  <si>
-    <t>88012486</t>
-  </si>
-  <si>
-    <t>88012487</t>
-  </si>
-  <si>
-    <t>88012491</t>
-  </si>
-  <si>
-    <t>88012498</t>
-  </si>
-  <si>
-    <t>88012499</t>
-  </si>
-  <si>
-    <t>88012500</t>
-  </si>
-  <si>
-    <t>88012511</t>
-  </si>
-  <si>
     <t>88012512</t>
   </si>
   <si>
     <t>88012513</t>
-  </si>
-  <si>
-    <t>88012668</t>
-  </si>
-  <si>
-    <t>88012669</t>
-  </si>
-  <si>
-    <t>88012670</t>
   </si>
   <si>
     <t>88012671</t>
@@ -121,7 +67,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -191,23 +136,23 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -224,10 +169,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -262,7 +207,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -297,7 +242,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -391,21 +336,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -422,7 +367,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -474,27 +419,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="2" max="3" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -523,7 +468,7 @@
         <v>2</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -531,7 +476,7 @@
         <v>21331512</v>
       </c>
       <c r="C2" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
@@ -544,27 +489,27 @@
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -598,10 +543,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="3">
-        <v>21331512</v>
+        <v>10817056</v>
       </c>
       <c r="C2" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
@@ -623,7 +568,7 @@
         <v>24561648</v>
       </c>
       <c r="C3" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
@@ -636,25 +581,25 @@
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -688,32 +633,32 @@
         <v>3</v>
       </c>
       <c r="B2" s="3">
-        <v>21331512</v>
+        <v>91327491</v>
       </c>
       <c r="C2" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="3">
-        <v>558</v>
+        <v>83</v>
       </c>
       <c r="F2" s="3">
-        <v>18052</v>
+        <v>89109</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -721,6 +666,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -793,6 +741,6 @@
       <c r="H3" s="3"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test Data - Update
</commit_message>
<xml_diff>
--- a/TestData/TestDataFile.xlsx
+++ b/TestData/TestDataFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="BOPIS_TestData" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="12">
   <si>
     <t>Item</t>
   </si>
@@ -54,13 +54,10 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>88012512</t>
-  </si>
-  <si>
-    <t>88012513</t>
-  </si>
-  <si>
-    <t>88012671</t>
+    <t>Ship To Store</t>
+  </si>
+  <si>
+    <t>Ship To Address</t>
   </si>
 </sst>
 </file>
@@ -429,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,7 +470,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3">
-        <v>21331512</v>
+        <v>29042081</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
@@ -488,9 +485,7 @@
         <v>18052</v>
       </c>
       <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="H2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -503,7 +498,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,13 +538,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="3">
-        <v>10817056</v>
+        <v>34174229</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3">
         <v>558</v>
@@ -571,7 +566,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3">
         <v>558</v>
@@ -580,9 +575,7 @@
         <v>18052</v>
       </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="H3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -593,12 +586,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -639,7 +633,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" s="3">
         <v>83</v>
@@ -648,9 +642,7 @@
         <v>89109</v>
       </c>
       <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Refactored the code and moved re-usable code to "AppGenericFunctions" class.
</commit_message>
<xml_diff>
--- a/TestData/TestDataFile.xlsx
+++ b/TestData/TestDataFile.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="BOPIS_TestData" sheetId="1" r:id="rId1"/>
-    <sheet name="SFS_TestData" sheetId="2" r:id="rId2"/>
-    <sheet name="STS_TestData" sheetId="3" r:id="rId3"/>
-    <sheet name="BackUp" sheetId="4" r:id="rId4"/>
+    <sheet name="BOPIS_TestData" r:id="rId1" sheetId="1"/>
+    <sheet name="SFS_TestData" r:id="rId2" sheetId="2"/>
+    <sheet name="STS_TestData" r:id="rId3" sheetId="3"/>
+    <sheet name="BackUp" r:id="rId4" sheetId="4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
   <si>
     <t>Item</t>
   </si>
@@ -58,12 +58,25 @@
   </si>
   <si>
     <t>Ship To Address</t>
+  </si>
+  <si>
+    <t>88015868</t>
+  </si>
+  <si>
+    <t>88015890</t>
+  </si>
+  <si>
+    <t>88015894</t>
+  </si>
+  <si>
+    <t>88015899</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -133,23 +146,23 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -166,10 +179,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -204,7 +217,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -239,7 +252,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -333,21 +346,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -364,7 +377,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -416,14 +429,178 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row customFormat="1" r="2" s="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3">
+        <v>29042081</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3">
+        <v>558</v>
+      </c>
+      <c r="F2" s="3">
+        <v>18052</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3">
+        <v>34174229</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3">
+        <v>558</v>
+      </c>
+      <c r="F2" s="3">
+        <v>18052</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3">
+        <v>24561648</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3">
+        <v>558</v>
+      </c>
+      <c r="F3" s="3">
+        <v>18052</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -432,11 +609,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -465,174 +639,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3">
-        <v>29042081</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3">
-        <v>558</v>
-      </c>
-      <c r="F2" s="3">
-        <v>18052</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3">
-        <v>34174229</v>
+        <v>91327491</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="3">
-        <v>558</v>
-      </c>
-      <c r="F2" s="3">
-        <v>18052</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3">
-        <v>24561648</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="3">
-        <v>558</v>
-      </c>
-      <c r="F3" s="3">
-        <v>18052</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3">
-        <v>91327491</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="3">
@@ -642,15 +659,17 @@
         <v>89109</v>
       </c>
       <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -659,7 +678,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -733,6 +752,6 @@
       <c r="H3" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Amex Card as payment --> App Generic Function has been added.
</commit_message>
<xml_diff>
--- a/TestData/TestDataFile.xlsx
+++ b/TestData/TestDataFile.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="17">
   <si>
     <t>Item</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>88015899</t>
+  </si>
+  <si>
+    <t>88015908</t>
   </si>
 </sst>
 </file>
@@ -660,7 +663,7 @@
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added code for Appeasement code selection..
</commit_message>
<xml_diff>
--- a/TestData/TestDataFile.xlsx
+++ b/TestData/TestDataFile.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="18">
   <si>
     <t>Item</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>88015908</t>
+  </si>
+  <si>
+    <t>88015910</t>
   </si>
 </sst>
 </file>
@@ -663,7 +666,7 @@
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scenario 15 - Completed
</commit_message>
<xml_diff>
--- a/TestData/TestDataFile.xlsx
+++ b/TestData/TestDataFile.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="23">
   <si>
     <t>Item</t>
   </si>
@@ -76,6 +76,21 @@
   </si>
   <si>
     <t>88015910</t>
+  </si>
+  <si>
+    <t>88015998</t>
+  </si>
+  <si>
+    <t>88016001</t>
+  </si>
+  <si>
+    <t>88016005</t>
+  </si>
+  <si>
+    <t>88016007</t>
+  </si>
+  <si>
+    <t>88016008</t>
   </si>
 </sst>
 </file>
@@ -666,7 +681,7 @@
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Screenshot capture method has been moved to Generic Functions
</commit_message>
<xml_diff>
--- a/TestData/TestDataFile.xlsx
+++ b/TestData/TestDataFile.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
   <si>
     <t>Item</t>
   </si>
@@ -91,6 +91,30 @@
   </si>
   <si>
     <t>88016008</t>
+  </si>
+  <si>
+    <t>88016056</t>
+  </si>
+  <si>
+    <t>88016064</t>
+  </si>
+  <si>
+    <t>88016067</t>
+  </si>
+  <si>
+    <t>88016070</t>
+  </si>
+  <si>
+    <t>88016071</t>
+  </si>
+  <si>
+    <t>88016075</t>
+  </si>
+  <si>
+    <t>88016077</t>
+  </si>
+  <si>
+    <t>88016078</t>
   </si>
 </sst>
 </file>
@@ -681,7 +705,7 @@
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moveToElement reusable function has been modified.
</commit_message>
<xml_diff>
--- a/TestData/TestDataFile.xlsx
+++ b/TestData/TestDataFile.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
   <si>
     <t>Item</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>88016133</t>
+  </si>
+  <si>
+    <t>88016551</t>
   </si>
 </sst>
 </file>
@@ -651,7 +654,7 @@
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>